<commit_message>
Toma datos del excel
</commit_message>
<xml_diff>
--- a/Resumen.xlsx
+++ b/Resumen.xlsx
@@ -7,6 +7,7 @@
   </bookViews>
   <sheets>
     <sheet name="Resumen" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Graficos" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="191029" fullCalcOnLoad="1"/>
@@ -18,7 +19,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="00"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="9">
     <font>
       <name val="Arial"/>
       <color rgb="FF000000"/>
@@ -65,8 +66,11 @@
       <color theme="1"/>
       <sz val="10"/>
     </font>
+    <font>
+      <b val="1"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="8">
     <fill>
       <patternFill/>
     </fill>
@@ -95,6 +99,18 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFFFF"/>
         <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00C4D79B"/>
+        <bgColor rgb="00C4D79B"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00EBF1DE"/>
+        <bgColor rgb="00EBF1DE"/>
       </patternFill>
     </fill>
   </fills>
@@ -208,7 +224,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="5" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -308,6 +324,10 @@
     <xf numFmtId="49" fontId="2" fillId="2" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="center" textRotation="90" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -455,7 +475,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:t/>
+                  <a:t>None</a:t>
                 </a:r>
                 <a:endParaRPr lang="es-AR"/>
               </a:p>
@@ -480,7 +500,7 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:t/>
+              <a:t>None</a:t>
             </a:r>
             <a:endParaRPr lang="es-AR"/>
           </a:p>
@@ -530,7 +550,7 @@
             </a:defRPr>
           </a:pPr>
           <a:r>
-            <a:t/>
+            <a:t>None</a:t>
           </a:r>
           <a:endParaRPr lang="es-AR"/>
         </a:p>
@@ -613,7 +633,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:t/>
+                  <a:t>None</a:t>
                 </a:r>
                 <a:endParaRPr lang="es-AR"/>
               </a:p>
@@ -638,7 +658,7 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:t/>
+              <a:t>None</a:t>
             </a:r>
             <a:endParaRPr lang="es-AR"/>
           </a:p>
@@ -688,7 +708,7 @@
             </a:defRPr>
           </a:pPr>
           <a:r>
-            <a:t/>
+            <a:t>None</a:t>
           </a:r>
           <a:endParaRPr lang="es-AR"/>
         </a:p>
@@ -696,6 +716,230 @@
     </legend>
     <plotVisOnly val="1"/>
     <dispBlanksAs val="zero"/>
+  </chart>
+</chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <chart>
+    <title>
+      <tx>
+        <rich>
+          <a:bodyPr/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:t>Cantidad de artículos por Año</a:t>
+            </a:r>
+          </a:p>
+        </rich>
+      </tx>
+    </title>
+    <plotArea>
+      <barChart>
+        <barDir val="col"/>
+        <grouping val="clustered"/>
+        <ser>
+          <idx val="0"/>
+          <order val="0"/>
+          <tx>
+            <strRef>
+              <f>'Graficos'!B2</f>
+            </strRef>
+          </tx>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <cat>
+            <numRef>
+              <f>'Graficos'!$A$3:$A$10</f>
+            </numRef>
+          </cat>
+          <val>
+            <numRef>
+              <f>'Graficos'!$B$3:$B$10</f>
+            </numRef>
+          </val>
+        </ser>
+        <gapWidth val="150"/>
+        <axId val="10"/>
+        <axId val="100"/>
+      </barChart>
+      <catAx>
+        <axId val="10"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <title>
+          <tx>
+            <rich>
+              <a:bodyPr/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:t>Año</a:t>
+                </a:r>
+              </a:p>
+            </rich>
+          </tx>
+        </title>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="100"/>
+        <lblOffset val="100"/>
+      </catAx>
+      <valAx>
+        <axId val="100"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <majorGridlines/>
+        <title>
+          <tx>
+            <rich>
+              <a:bodyPr/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:t>Cantidad</a:t>
+                </a:r>
+              </a:p>
+            </rich>
+          </tx>
+        </title>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="10"/>
+      </valAx>
+    </plotArea>
+    <legend>
+      <legendPos val="r"/>
+    </legend>
+    <plotVisOnly val="1"/>
+    <dispBlanksAs val="gap"/>
+  </chart>
+</chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <chart>
+    <title>
+      <tx>
+        <rich>
+          <a:bodyPr/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:t>Cantidad de artículos por País</a:t>
+            </a:r>
+          </a:p>
+        </rich>
+      </tx>
+    </title>
+    <plotArea>
+      <barChart>
+        <barDir val="col"/>
+        <grouping val="clustered"/>
+        <ser>
+          <idx val="0"/>
+          <order val="0"/>
+          <tx>
+            <strRef>
+              <f>'Graficos'!B32</f>
+            </strRef>
+          </tx>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <cat>
+            <numRef>
+              <f>'Graficos'!$A$33:$A$39</f>
+            </numRef>
+          </cat>
+          <val>
+            <numRef>
+              <f>'Graficos'!$B$33:$B$39</f>
+            </numRef>
+          </val>
+        </ser>
+        <gapWidth val="150"/>
+        <axId val="10"/>
+        <axId val="100"/>
+      </barChart>
+      <catAx>
+        <axId val="10"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <title>
+          <tx>
+            <rich>
+              <a:bodyPr/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:t>País</a:t>
+                </a:r>
+              </a:p>
+            </rich>
+          </tx>
+        </title>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="100"/>
+        <lblOffset val="100"/>
+      </catAx>
+      <valAx>
+        <axId val="100"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <majorGridlines/>
+        <title>
+          <tx>
+            <rich>
+              <a:bodyPr/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:t>Cantidad</a:t>
+                </a:r>
+              </a:p>
+            </rich>
+          </tx>
+        </title>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="10"/>
+      </valAx>
+    </plotArea>
+    <legend>
+      <legendPos val="r"/>
+    </legend>
+    <plotVisOnly val="1"/>
+    <dispBlanksAs val="gap"/>
   </chart>
 </chartSpace>
 </file>
@@ -745,6 +989,55 @@
       </a:graphic>
     </graphicFrame>
     <clientData fLocksWithSheet="0"/>
+  </oneCellAnchor>
+</wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <oneCellAnchor>
+    <from>
+      <col>4</col>
+      <colOff>0</colOff>
+      <row>1</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="5400000" cy="2700000"/>
+    <graphicFrame>
+      <nvGraphicFramePr>
+        <cNvPr id="1" name="Chart 1"/>
+        <cNvGraphicFramePr/>
+      </nvGraphicFramePr>
+      <xfrm/>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </graphicFrame>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>4</col>
+      <colOff>0</colOff>
+      <row>31</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="5400000" cy="2700000"/>
+    <graphicFrame>
+      <nvGraphicFramePr>
+        <cNvPr id="2" name="Chart 2"/>
+        <cNvGraphicFramePr/>
+      </nvGraphicFramePr>
+      <xfrm/>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </graphicFrame>
+    <clientData/>
   </oneCellAnchor>
 </wsDr>
 </file>
@@ -960,7 +1253,7 @@
       <selection pane="bottomRight" activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col width="5" customWidth="1" min="1" max="1"/>
     <col width="26.42578125" customWidth="1" min="2" max="2"/>
@@ -992,16 +1285,36 @@
       <c r="E1" s="7" t="n">
         <v>2</v>
       </c>
-      <c r="F1" s="7" t="n"/>
-      <c r="G1" s="7" t="n"/>
-      <c r="H1" s="7" t="n"/>
-      <c r="I1" s="7" t="n"/>
-      <c r="J1" s="7" t="n"/>
-      <c r="K1" s="7" t="n"/>
-      <c r="L1" s="7" t="n"/>
-      <c r="M1" s="7" t="n"/>
-      <c r="N1" s="7" t="n"/>
-      <c r="O1" s="7" t="n"/>
+      <c r="F1" s="7" t="n">
+        <v>3</v>
+      </c>
+      <c r="G1" s="7" t="n">
+        <v>4</v>
+      </c>
+      <c r="H1" s="7" t="n">
+        <v>5</v>
+      </c>
+      <c r="I1" s="7" t="n">
+        <v>6</v>
+      </c>
+      <c r="J1" s="7" t="n">
+        <v>7</v>
+      </c>
+      <c r="K1" s="7" t="n">
+        <v>8</v>
+      </c>
+      <c r="L1" s="7" t="n">
+        <v>9</v>
+      </c>
+      <c r="M1" s="7" t="n">
+        <v>10</v>
+      </c>
+      <c r="N1" s="7" t="n">
+        <v>11</v>
+      </c>
+      <c r="O1" s="7" t="n">
+        <v>12</v>
+      </c>
       <c r="P1" s="7" t="n"/>
       <c r="Q1" s="7" t="n"/>
       <c r="R1" s="8" t="n"/>
@@ -1040,16 +1353,56 @@
           <t>https://ieeexplore.ieee.org/document/4053283</t>
         </is>
       </c>
-      <c r="F2" s="15" t="n"/>
-      <c r="G2" s="16" t="n"/>
-      <c r="H2" s="15" t="n"/>
-      <c r="I2" s="15" t="n"/>
-      <c r="J2" s="16" t="n"/>
-      <c r="K2" s="15" t="n"/>
-      <c r="L2" s="15" t="n"/>
-      <c r="M2" s="15" t="n"/>
-      <c r="N2" s="15" t="n"/>
-      <c r="O2" s="15" t="n"/>
+      <c r="F2" s="15" t="inlineStr">
+        <is>
+          <t>https://ieeexplore.ieee.org/document/10993799</t>
+        </is>
+      </c>
+      <c r="G2" s="16" t="inlineStr">
+        <is>
+          <t>https://ieeexplore.ieee.org/document/8397647</t>
+        </is>
+      </c>
+      <c r="H2" s="15" t="inlineStr">
+        <is>
+          <t>https://ieeexplore.ieee.org/document/6493605</t>
+        </is>
+      </c>
+      <c r="I2" s="15" t="inlineStr">
+        <is>
+          <t>https://ieeexplore.ieee.org/document/10270721</t>
+        </is>
+      </c>
+      <c r="J2" s="16" t="inlineStr">
+        <is>
+          <t>https://ieeexplore.ieee.org/document/10121659</t>
+        </is>
+      </c>
+      <c r="K2" s="15" t="inlineStr">
+        <is>
+          <t>https://ieeexplore.ieee.org/document/9006200</t>
+        </is>
+      </c>
+      <c r="L2" s="15" t="inlineStr">
+        <is>
+          <t>https://ieeexplore.ieee.org/document/10158172</t>
+        </is>
+      </c>
+      <c r="M2" s="15" t="inlineStr">
+        <is>
+          <t>https://ieeexplore.ieee.org/document/10423308</t>
+        </is>
+      </c>
+      <c r="N2" s="15" t="inlineStr">
+        <is>
+          <t>https://ieeexplore.ieee.org/document/9842688</t>
+        </is>
+      </c>
+      <c r="O2" s="15" t="inlineStr">
+        <is>
+          <t>https://ieeexplore.ieee.org/document/9006051</t>
+        </is>
+      </c>
       <c r="P2" s="15" t="n"/>
       <c r="Q2" s="15" t="n"/>
       <c r="R2" s="15" t="n"/>
@@ -1084,16 +1437,56 @@
           <t>Active: A Unified Platform for Building Intelligent Web Interaction Assistants</t>
         </is>
       </c>
-      <c r="F3" s="21" t="n"/>
-      <c r="G3" s="21" t="n"/>
-      <c r="H3" s="21" t="n"/>
-      <c r="I3" s="21" t="n"/>
-      <c r="J3" s="21" t="n"/>
-      <c r="K3" s="21" t="n"/>
-      <c r="L3" s="3" t="n"/>
-      <c r="M3" s="3" t="n"/>
-      <c r="N3" s="19" t="n"/>
-      <c r="O3" s="3" t="n"/>
+      <c r="F3" s="21" t="inlineStr">
+        <is>
+          <t>Integrating Spring Boot with Cloud Services for Scalable Java Applications with the test results of AI Implementation</t>
+        </is>
+      </c>
+      <c r="G3" s="21" t="inlineStr">
+        <is>
+          <t>Workload performance and interference on containers</t>
+        </is>
+      </c>
+      <c r="H3" s="21" t="inlineStr">
+        <is>
+          <t>Transactional Memory Architecture and Implementation for IBM System Z</t>
+        </is>
+      </c>
+      <c r="I3" s="21" t="inlineStr">
+        <is>
+          <t>Comparing Microservices and Monolithic Applications in a DevOps Context</t>
+        </is>
+      </c>
+      <c r="J3" s="21" t="inlineStr">
+        <is>
+          <t>CfgNet: A Framework for Tracking Equality-Based Configuration Dependencies Across a Software Project</t>
+        </is>
+      </c>
+      <c r="K3" s="21" t="inlineStr">
+        <is>
+          <t>Paper Recommendation Based on Citation Relation</t>
+        </is>
+      </c>
+      <c r="L3" s="3" t="inlineStr">
+        <is>
+          <t>Application of Software Engineering Technology in System Software Development</t>
+        </is>
+      </c>
+      <c r="M3" s="3" t="inlineStr">
+        <is>
+          <t>Agile development research based on software engineering to software testing</t>
+        </is>
+      </c>
+      <c r="N3" s="19" t="inlineStr">
+        <is>
+          <t>Customer Support In The Era of Continuous Deployment: A Software-Intensive Embedded Systems Case Study</t>
+        </is>
+      </c>
+      <c r="O3" s="3" t="inlineStr">
+        <is>
+          <t>Big Federal Data Centers Implementing FAIR Data Principles: ARM Data Center Example</t>
+        </is>
+      </c>
       <c r="P3" s="19" t="n"/>
       <c r="Q3" s="19" t="n"/>
       <c r="R3" s="19" t="n"/>
@@ -1128,16 +1521,56 @@
           <t>Guzzoni, Didier and Baur, Charles and Cheyer, Adam</t>
         </is>
       </c>
-      <c r="F4" s="21" t="n"/>
-      <c r="G4" s="21" t="n"/>
-      <c r="H4" s="21" t="n"/>
-      <c r="I4" s="21" t="n"/>
-      <c r="J4" s="21" t="n"/>
-      <c r="K4" s="21" t="n"/>
-      <c r="L4" s="3" t="n"/>
-      <c r="M4" s="3" t="n"/>
-      <c r="N4" s="19" t="n"/>
-      <c r="O4" s="3" t="n"/>
+      <c r="F4" s="21" t="inlineStr">
+        <is>
+          <t>Aladiyan, Anbarasu</t>
+        </is>
+      </c>
+      <c r="G4" s="21" t="inlineStr">
+        <is>
+          <t>Garg, Surya Kant and Lakshmi, J.</t>
+        </is>
+      </c>
+      <c r="H4" s="21" t="inlineStr">
+        <is>
+          <t>Jacobi, Christian and Slegel, Timothy and Greiner, Dan</t>
+        </is>
+      </c>
+      <c r="I4" s="21" t="inlineStr">
+        <is>
+          <t>Chouhan, Utkarsh and Tiwari, Vaibhav and Kumar, Hradesh</t>
+        </is>
+      </c>
+      <c r="J4" s="21" t="inlineStr">
+        <is>
+          <t>Simon, Sebastian and Ruckel, Nicolai and Siegmund, Norbert</t>
+        </is>
+      </c>
+      <c r="K4" s="21" t="inlineStr">
+        <is>
+          <t>Tanner, William and Akbas, Esra and Hasan, Mir</t>
+        </is>
+      </c>
+      <c r="L4" s="3" t="inlineStr">
+        <is>
+          <t>Zhao, Chenxiao and Wang, Yu and Jiang, Jingjing</t>
+        </is>
+      </c>
+      <c r="M4" s="3" t="inlineStr">
+        <is>
+          <t>Chen, QiaoLi and Guo, LiWen and Feng, YunChen</t>
+        </is>
+      </c>
+      <c r="N4" s="19" t="inlineStr">
+        <is>
+          <t>Dakkak, Anas and Munappy, Aiswarya Raj and Bosch, Jan and Olsson, Helena Hölmstrom</t>
+        </is>
+      </c>
+      <c r="O4" s="3" t="inlineStr">
+        <is>
+          <t>Devarakonda, Ranjeet and Prakash, Giri and Guntupally, Kavya and Kumar, Jitendra</t>
+        </is>
+      </c>
       <c r="P4" s="19" t="n"/>
       <c r="Q4" s="19" t="n"/>
       <c r="R4" s="19" t="n"/>
@@ -1168,16 +1601,36 @@
       <c r="E5" s="19" t="n">
         <v>2006</v>
       </c>
-      <c r="F5" s="19" t="n"/>
-      <c r="G5" s="19" t="n"/>
-      <c r="H5" s="19" t="n"/>
-      <c r="I5" s="19" t="n"/>
-      <c r="J5" s="19" t="n"/>
-      <c r="K5" s="19" t="n"/>
-      <c r="L5" s="3" t="n"/>
-      <c r="M5" s="3" t="n"/>
-      <c r="N5" s="19" t="n"/>
-      <c r="O5" s="3" t="n"/>
+      <c r="F5" s="19" t="n">
+        <v>2024</v>
+      </c>
+      <c r="G5" s="19" t="n">
+        <v>2017</v>
+      </c>
+      <c r="H5" s="19" t="n">
+        <v>2012</v>
+      </c>
+      <c r="I5" s="19" t="n">
+        <v>2023</v>
+      </c>
+      <c r="J5" s="19" t="n">
+        <v>2023</v>
+      </c>
+      <c r="K5" s="19" t="n">
+        <v>2019</v>
+      </c>
+      <c r="L5" s="3" t="n">
+        <v>2023</v>
+      </c>
+      <c r="M5" s="3" t="n">
+        <v>2023</v>
+      </c>
+      <c r="N5" s="19" t="n">
+        <v>2022</v>
+      </c>
+      <c r="O5" s="3" t="n">
+        <v>2019</v>
+      </c>
       <c r="P5" s="19" t="n"/>
       <c r="Q5" s="19" t="n"/>
       <c r="R5" s="19" t="n"/>
@@ -1248,16 +1701,56 @@
           <t>IEEE</t>
         </is>
       </c>
-      <c r="F7" s="19" t="n"/>
-      <c r="G7" s="19" t="n"/>
-      <c r="H7" s="19" t="n"/>
-      <c r="I7" s="19" t="n"/>
-      <c r="J7" s="19" t="n"/>
-      <c r="K7" s="19" t="n"/>
-      <c r="L7" s="3" t="n"/>
-      <c r="M7" s="3" t="n"/>
-      <c r="N7" s="19" t="n"/>
-      <c r="O7" s="3" t="n"/>
+      <c r="F7" s="19" t="inlineStr">
+        <is>
+          <t>IEEE</t>
+        </is>
+      </c>
+      <c r="G7" s="19" t="inlineStr">
+        <is>
+          <t>IEEE</t>
+        </is>
+      </c>
+      <c r="H7" s="19" t="inlineStr">
+        <is>
+          <t>IEEE</t>
+        </is>
+      </c>
+      <c r="I7" s="19" t="inlineStr">
+        <is>
+          <t>IEEE</t>
+        </is>
+      </c>
+      <c r="J7" s="19" t="inlineStr">
+        <is>
+          <t>IEEE</t>
+        </is>
+      </c>
+      <c r="K7" s="19" t="inlineStr">
+        <is>
+          <t>IEEE</t>
+        </is>
+      </c>
+      <c r="L7" s="3" t="inlineStr">
+        <is>
+          <t>IEEE</t>
+        </is>
+      </c>
+      <c r="M7" s="3" t="inlineStr">
+        <is>
+          <t>IEEE</t>
+        </is>
+      </c>
+      <c r="N7" s="19" t="inlineStr">
+        <is>
+          <t>IEEE</t>
+        </is>
+      </c>
+      <c r="O7" s="3" t="inlineStr">
+        <is>
+          <t>IEEE</t>
+        </is>
+      </c>
       <c r="P7" s="19" t="n"/>
       <c r="Q7" s="19" t="n"/>
       <c r="R7" s="19" t="n"/>
@@ -1292,16 +1785,52 @@
           <t>2006 IEEE/WIC/ACM International Conference on Web Intelligence and Intelligent Agent Technology Workshops</t>
         </is>
       </c>
-      <c r="F8" s="19" t="n"/>
-      <c r="G8" s="19" t="n"/>
-      <c r="H8" s="19" t="n"/>
-      <c r="I8" s="19" t="n"/>
-      <c r="J8" s="19" t="n"/>
-      <c r="K8" s="19" t="n"/>
-      <c r="L8" s="19" t="n"/>
-      <c r="M8" s="19" t="n"/>
-      <c r="N8" s="19" t="n"/>
-      <c r="O8" s="3" t="n"/>
+      <c r="F8" s="19" t="inlineStr">
+        <is>
+          <t>2024 International Conference on Communication, Computing and Energy Efficient Technologies (I3CEET)</t>
+        </is>
+      </c>
+      <c r="G8" s="19" t="inlineStr">
+        <is>
+          <t>2017 IEEE SmartWorld, Ubiquitous Intelligence &amp; Computing, Advanced &amp; Trusted Computed, Scalable Computing &amp; Communications, Cloud &amp; Big Data Computing, Internet of People and Smart City Innovation (SmartWorld/SCALCOM/UIC/ATC/CBDCom/IOP/SCI)</t>
+        </is>
+      </c>
+      <c r="H8" s="19" t="inlineStr">
+        <is>
+          <t>2012 45th Annual IEEE/ACM International Symposium on Microarchitecture</t>
+        </is>
+      </c>
+      <c r="I8" s="19" t="inlineStr">
+        <is>
+          <t>2023 3rd Asian Conference on Innovation in Technology (ASIANCON)</t>
+        </is>
+      </c>
+      <c r="J8" s="19" t="inlineStr"/>
+      <c r="K8" s="19" t="inlineStr">
+        <is>
+          <t>2019 IEEE International Conference on Big Data (Big Data)</t>
+        </is>
+      </c>
+      <c r="L8" s="19" t="inlineStr">
+        <is>
+          <t>2023 Asia-Europe Conference on Electronics, Data Processing and Informatics (ACEDPI)</t>
+        </is>
+      </c>
+      <c r="M8" s="19" t="inlineStr">
+        <is>
+          <t>2023 9th International Conference on Systems and Informatics (ICSAI)</t>
+        </is>
+      </c>
+      <c r="N8" s="19" t="inlineStr">
+        <is>
+          <t>2022 IEEE 46th Annual Computers, Software, and Applications Conference (COMPSAC)</t>
+        </is>
+      </c>
+      <c r="O8" s="3" t="inlineStr">
+        <is>
+          <t>2019 IEEE International Conference on Big Data (Big Data)</t>
+        </is>
+      </c>
       <c r="P8" s="19" t="n"/>
       <c r="Q8" s="19" t="n"/>
       <c r="R8" s="19" t="n"/>
@@ -1336,16 +1865,56 @@
           <t>China</t>
         </is>
       </c>
-      <c r="F9" s="19" t="n"/>
-      <c r="G9" s="19" t="n"/>
-      <c r="H9" s="19" t="n"/>
-      <c r="I9" s="19" t="n"/>
-      <c r="J9" s="19" t="n"/>
-      <c r="K9" s="19" t="n"/>
-      <c r="L9" s="3" t="n"/>
-      <c r="M9" s="3" t="n"/>
-      <c r="N9" s="19" t="n"/>
-      <c r="O9" s="3" t="n"/>
+      <c r="F9" s="19" t="inlineStr">
+        <is>
+          <t>India</t>
+        </is>
+      </c>
+      <c r="G9" s="19" t="inlineStr">
+        <is>
+          <t>USA</t>
+        </is>
+      </c>
+      <c r="H9" s="19" t="inlineStr">
+        <is>
+          <t>Canada</t>
+        </is>
+      </c>
+      <c r="I9" s="19" t="inlineStr">
+        <is>
+          <t>India</t>
+        </is>
+      </c>
+      <c r="J9" s="19" t="inlineStr">
+        <is>
+          <t>No Disponible</t>
+        </is>
+      </c>
+      <c r="K9" s="19" t="inlineStr">
+        <is>
+          <t>USA</t>
+        </is>
+      </c>
+      <c r="L9" s="3" t="inlineStr">
+        <is>
+          <t>Czech Republic</t>
+        </is>
+      </c>
+      <c r="M9" s="3" t="inlineStr">
+        <is>
+          <t>China</t>
+        </is>
+      </c>
+      <c r="N9" s="19" t="inlineStr">
+        <is>
+          <t>USA</t>
+        </is>
+      </c>
+      <c r="O9" s="3" t="inlineStr">
+        <is>
+          <t>USA</t>
+        </is>
+      </c>
       <c r="P9" s="19" t="n"/>
       <c r="Q9" s="19" t="n"/>
       <c r="R9" s="19" t="n"/>
@@ -1376,16 +1945,36 @@
       <c r="E10" s="19" t="n">
         <v>195</v>
       </c>
-      <c r="F10" s="19" t="n"/>
-      <c r="G10" s="19" t="n"/>
-      <c r="H10" s="19" t="n"/>
-      <c r="I10" s="19" t="n"/>
-      <c r="J10" s="19" t="n"/>
-      <c r="K10" s="19" t="n"/>
-      <c r="L10" s="3" t="n"/>
-      <c r="M10" s="3" t="n"/>
-      <c r="N10" s="19" t="n"/>
-      <c r="O10" s="3" t="n"/>
+      <c r="F10" s="19" t="n">
+        <v>0</v>
+      </c>
+      <c r="G10" s="19" t="n">
+        <v>7</v>
+      </c>
+      <c r="H10" s="19" t="n">
+        <v>139</v>
+      </c>
+      <c r="I10" s="19" t="n">
+        <v>2</v>
+      </c>
+      <c r="J10" s="19" t="n">
+        <v>2</v>
+      </c>
+      <c r="K10" s="19" t="n">
+        <v>15</v>
+      </c>
+      <c r="L10" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="M10" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="N10" s="19" t="n">
+        <v>2</v>
+      </c>
+      <c r="O10" s="3" t="n">
+        <v>8</v>
+      </c>
       <c r="P10" s="19" t="n"/>
       <c r="Q10" s="19" t="n"/>
       <c r="R10" s="19" t="n"/>
@@ -1420,16 +2009,52 @@
           <t>Intelligent structures;Artificial intelligence;Application software;Information retrieval;Intelligent agent;Intelligent robots;Software tools;Natural languages;Computer architecture;Laboratories</t>
         </is>
       </c>
-      <c r="F11" s="19" t="n"/>
-      <c r="G11" s="19" t="n"/>
-      <c r="H11" s="19" t="n"/>
-      <c r="I11" s="19" t="n"/>
-      <c r="J11" s="19" t="n"/>
-      <c r="K11" s="19" t="n"/>
-      <c r="L11" s="3" t="n"/>
-      <c r="M11" s="3" t="n"/>
-      <c r="N11" s="19" t="n"/>
-      <c r="O11" s="3" t="n"/>
+      <c r="F11" s="19" t="inlineStr">
+        <is>
+          <t>Cloud computing;Java;Scalability;Software as a service;Microservice architectures;Serverless computing;Computer architecture;Complexity theory;Security;Artificial intelligence;Abstract: AI Implementation testing result;Cloud Computing;Spring Boot;Java Applications;Scalability;Microservices Architecture;Cloud-Native;AWS;Google Cloud Platform;Azure;Serverless Computing;CI/CD</t>
+        </is>
+      </c>
+      <c r="G11" s="19" t="inlineStr">
+        <is>
+          <t>Containers;Servers;Kernel;Linux;Interference;Benchmark testing;Resource management</t>
+        </is>
+      </c>
+      <c r="H11" s="19" t="inlineStr"/>
+      <c r="I11" s="19" t="inlineStr">
+        <is>
+          <t>Technological innovation;Microservice architectures;Organizations;Best practices;Testing;Monolithic Architecture;Microservice Architecture;DevOps;Agile;CI/CD</t>
+        </is>
+      </c>
+      <c r="J11" s="19" t="inlineStr">
+        <is>
+          <t>Software;Java;Codes;Pipelines;Software systems;Software development management;Security;Configuration dependencies;configuration conflicts;services and components</t>
+        </is>
+      </c>
+      <c r="K11" s="19" t="inlineStr">
+        <is>
+          <t>Collaboration;Portable document format;Metadata;Google;Measurement;Couplings;Citation analysis;Citation networks;recommendation systems;scholarly data;paper recommendation;network science</t>
+        </is>
+      </c>
+      <c r="L11" s="3" t="inlineStr">
+        <is>
+          <t>Data processing;Data models;System software;Informatics;Consumer electronics;Software engineering;Software development management;software engineering;software development;key points of application</t>
+        </is>
+      </c>
+      <c r="M11" s="3" t="inlineStr">
+        <is>
+          <t>Software testing;Software quality;Market research;User experience;Scrum (Software development);Task analysis;Software engineering;Agile Development model;XP approach;Scrum model;test-driven development (TDD);automated testing techniques;CDIO</t>
+        </is>
+      </c>
+      <c r="N11" s="19" t="inlineStr">
+        <is>
+          <t>Fault diagnosis;Embedded systems;Conferences;Sociology;Collaboration;Companies;Software;Software-intensive embedded system;Continu-ous Deployment;Customer Support</t>
+        </is>
+      </c>
+      <c r="O11" s="3" t="inlineStr">
+        <is>
+          <t>Metadata;Data centers;Big Data;Tools;Atmospheric measurements;Distributed databases;Big data;ARM Data Center;FAIR;scientific data mining;data management</t>
+        </is>
+      </c>
       <c r="P11" s="19" t="n"/>
       <c r="Q11" s="19" t="n"/>
       <c r="R11" s="19" t="n"/>
@@ -1466,16 +2091,64 @@
 keywords: {Intelligent structures;Artificial intelligence;Application software;Information retrieval;Intelligent agent;Intelligent robots;Software tools;Natural languages;Computer architecture;Laboratories},</t>
         </is>
       </c>
-      <c r="F12" s="21" t="n"/>
-      <c r="G12" s="21" t="n"/>
-      <c r="H12" s="21" t="n"/>
-      <c r="I12" s="21" t="n"/>
-      <c r="J12" s="21" t="n"/>
-      <c r="K12" s="21" t="n"/>
-      <c r="L12" s="3" t="n"/>
-      <c r="M12" s="3" t="n"/>
-      <c r="N12" s="19" t="n"/>
-      <c r="O12" s="26" t="n"/>
+      <c r="F12" s="21" t="inlineStr">
+        <is>
+          <t>A. Aladiyan, "Integrating Spring Boot with Cloud Services for Scalable Java Applications with the test results of AI Implementation," 2024 International Conference on Communication, Computing and Energy Efficient Technologies (I3CEET), Gautam Buddha Nagar, India, 2024, pp. 17-22, doi: 10.1109/I3CEET61722.2024.10993799.
+keywords: {Cloud computing;Java;Scalability;Software as a service;Microservice architectures;Serverless computing;Computer architecture;Complexity theory;Security;Artificial intelligence;Abstract: AI Implementation testing result;Cloud Computing;Spring Boot;Java Applications;Scalability;Microservices Architecture;Cloud-Native;AWS;Google Cloud Platform;Azure;Serverless Computing;CI/CD},</t>
+        </is>
+      </c>
+      <c r="G12" s="21" t="inlineStr">
+        <is>
+          <t>S. K. Garg and J. Lakshmi, "Workload performance and interference on containers," 2017 IEEE SmartWorld, Ubiquitous Intelligence &amp; Computing, Advanced &amp; Trusted Computed, Scalable Computing &amp; Communications, Cloud &amp; Big Data Computing, Internet of People and Smart City Innovation (SmartWorld/SCALCOM/UIC/ATC/CBDCom/IOP/SCI), San Francisco, CA, USA, 2017, pp. 1-6, doi: 10.1109/UIC-ATC.2017.8397647.
+keywords: {Containers;Servers;Kernel;Linux;Interference;Benchmark testing;Resource management},</t>
+        </is>
+      </c>
+      <c r="H12" s="21" t="inlineStr">
+        <is>
+          <t>C. Jacobi, T. Slegel and D. Greiner, "Transactional Memory Architecture and Implementation for IBM System Z," 2012 45th Annual IEEE/ACM International Symposium on Microarchitecture, Vancouver, BC, Canada, 2012, pp. 25-36, doi: 10.1109/MICRO.2012.12.</t>
+        </is>
+      </c>
+      <c r="I12" s="21" t="inlineStr">
+        <is>
+          <t>U. Chouhan, V. Tiwari and H. Kumar, "Comparing Microservices and Monolithic Applications in a DevOps Context," 2023 3rd Asian Conference on Innovation in Technology (ASIANCON), Ravet IN, India, 2023, pp. 1-7, doi: 10.1109/ASIANCON58793.2023.10270721.
+keywords: {Technological innovation;Microservice architectures;Organizations;Best practices;Testing;Monolithic Architecture;Microservice Architecture;DevOps;Agile;CI/CD},</t>
+        </is>
+      </c>
+      <c r="J12" s="21" t="inlineStr">
+        <is>
+          <t>S. Simon, N. Ruckel and N. Siegmund, "CfgNet: A Framework for Tracking Equality-Based Configuration Dependencies Across a Software Project," in IEEE Transactions on Software Engineering, vol. 49, no. 8, pp. 3955-3971, Aug. 2023, doi: 10.1109/TSE.2023.3274349. keywords: {Software;Java;Codes;Pipelines;Software systems;Software development management;Security;Configuration dependencies;configuration conflicts;services and components},</t>
+        </is>
+      </c>
+      <c r="K12" s="21" t="inlineStr">
+        <is>
+          <t>W. Tanner, E. Akbas and M. Hasan, "Paper Recommendation Based on Citation Relation," 2019 IEEE International Conference on Big Data (Big Data), Los Angeles, CA, USA, 2019, pp. 3053-3059, doi: 10.1109/BigData47090.2019.9006200.
+keywords: {Collaboration;Portable document format;Metadata;Google;Measurement;Couplings;Citation analysis;Citation networks;recommendation systems;scholarly data;paper recommendation;network science},</t>
+        </is>
+      </c>
+      <c r="L12" s="3" t="inlineStr">
+        <is>
+          <t>C. Zhao, Y. Wang and J. Jiang, "Application of Software Engineering Technology in System Software Development," 2023 Asia-Europe Conference on Electronics, Data Processing and Informatics (ACEDPI), Prague, Czech Republic, 2023, pp. 502-506, doi: 10.1109/ACEDPI58926.2023.00101.
+keywords: {Data processing;Data models;System software;Informatics;Consumer electronics;Software engineering;Software development management;software engineering;software development;key points of application},</t>
+        </is>
+      </c>
+      <c r="M12" s="3" t="inlineStr">
+        <is>
+          <t>Q. Chen, L. Guo and Y. Feng, "Agile development research based on software engineering to software testing," 2023 9th International Conference on Systems and Informatics (ICSAI), Changsha, China, 2023, pp. 1-3, doi: 10.1109/ICSAI61474.2023.10423308.
+keywords: {Software testing;Software quality;Market research;User experience;Scrum (Software development);Task analysis;Software engineering;Agile Development model;XP approach;Scrum model;test-driven development (TDD);automated testing techniques;CDIO},</t>
+        </is>
+      </c>
+      <c r="N12" s="19" t="inlineStr">
+        <is>
+          <t>A. Dakkak, A. R. Munappy, J. Bosch and H. H. Olsson, "Customer Support In The Era of Continuous Deployment: A Software-Intensive Embedded Systems Case Study," 2022 IEEE 46th Annual Computers, Software, and Applications Conference (COMPSAC), Los Alamitos, CA, USA, 2022, pp. 914-923, doi: 10.1109/COMPSAC54236.2022.00143.
+keywords: {Fault diagnosis;Embedded systems;Conferences;Sociology;Collaboration;Companies;Software;Software-intensive embedded system;Continu-ous Deployment;Customer Support},</t>
+        </is>
+      </c>
+      <c r="O12" s="26" t="inlineStr">
+        <is>
+          <t>R. Devarakonda, G. Prakash, K. Guntupally and J. Kumar, "Big Federal Data Centers Implementing FAIR Data Principles: ARM Data Center Example," 2019 IEEE International Conference on Big Data (Big Data), Los Angeles, CA, USA, 2019, pp. 6033-6036, doi: 10.1109/BigData47090.2019.9006051.
+keywords: {Metadata;Data centers;Big Data;Tools;Atmospheric measurements;Distributed databases;Big data;ARM Data Center;FAIR;scientific data mining;data management},</t>
+        </is>
+      </c>
       <c r="P12" s="19" t="n"/>
       <c r="Q12" s="15" t="n"/>
       <c r="R12" s="15" t="n"/>
@@ -1510,16 +2183,56 @@
           <t>10.1109/WI-IATW.2006.27</t>
         </is>
       </c>
-      <c r="F13" s="21" t="n"/>
-      <c r="G13" s="21" t="n"/>
-      <c r="H13" s="21" t="n"/>
-      <c r="I13" s="21" t="n"/>
-      <c r="J13" s="21" t="n"/>
-      <c r="K13" s="21" t="n"/>
-      <c r="L13" s="3" t="n"/>
-      <c r="M13" s="3" t="n"/>
-      <c r="N13" s="19" t="n"/>
-      <c r="O13" s="26" t="n"/>
+      <c r="F13" s="21" t="inlineStr">
+        <is>
+          <t>10.1109/I3CEET61722.2024.10993799</t>
+        </is>
+      </c>
+      <c r="G13" s="21" t="inlineStr">
+        <is>
+          <t>10.1109/UIC-ATC.2017.8397647</t>
+        </is>
+      </c>
+      <c r="H13" s="21" t="inlineStr">
+        <is>
+          <t>10.1109/MICRO.2012.12</t>
+        </is>
+      </c>
+      <c r="I13" s="21" t="inlineStr">
+        <is>
+          <t>10.1109/ASIANCON58793.2023.10270721</t>
+        </is>
+      </c>
+      <c r="J13" s="21" t="inlineStr">
+        <is>
+          <t>10.1109/TSE.2023.3274349</t>
+        </is>
+      </c>
+      <c r="K13" s="21" t="inlineStr">
+        <is>
+          <t>10.1109/BigData47090.2019.9006200</t>
+        </is>
+      </c>
+      <c r="L13" s="3" t="inlineStr">
+        <is>
+          <t>10.1109/ACEDPI58926.2023.00101</t>
+        </is>
+      </c>
+      <c r="M13" s="3" t="inlineStr">
+        <is>
+          <t>10.1109/ICSAI61474.2023.10423308</t>
+        </is>
+      </c>
+      <c r="N13" s="19" t="inlineStr">
+        <is>
+          <t>10.1109/COMPSAC54236.2022.00143</t>
+        </is>
+      </c>
+      <c r="O13" s="26" t="inlineStr">
+        <is>
+          <t>10.1109/BigData47090.2019.9006051</t>
+        </is>
+      </c>
       <c r="P13" s="19" t="n"/>
       <c r="Q13" s="15" t="n"/>
       <c r="R13" s="15" t="n"/>
@@ -1550,16 +2263,36 @@
       <c r="E14" s="21" t="n">
         <v>280</v>
       </c>
-      <c r="F14" s="21" t="n"/>
-      <c r="G14" s="21" t="n"/>
-      <c r="H14" s="21" t="n"/>
-      <c r="I14" s="21" t="n"/>
-      <c r="J14" s="21" t="n"/>
-      <c r="K14" s="21" t="n"/>
-      <c r="L14" s="3" t="n"/>
-      <c r="M14" s="3" t="n"/>
-      <c r="N14" s="19" t="n"/>
-      <c r="O14" s="26" t="n"/>
+      <c r="F14" s="21" t="n">
+        <v>80</v>
+      </c>
+      <c r="G14" s="21" t="n">
+        <v>554</v>
+      </c>
+      <c r="H14" s="21" t="n">
+        <v>663</v>
+      </c>
+      <c r="I14" s="21" t="n">
+        <v>200</v>
+      </c>
+      <c r="J14" s="21" t="n">
+        <v>476</v>
+      </c>
+      <c r="K14" s="21" t="n">
+        <v>694</v>
+      </c>
+      <c r="L14" s="3" t="n">
+        <v>482</v>
+      </c>
+      <c r="M14" s="3" t="n">
+        <v>630</v>
+      </c>
+      <c r="N14" s="19" t="n">
+        <v>237</v>
+      </c>
+      <c r="O14" s="26" t="n">
+        <v>797</v>
+      </c>
       <c r="P14" s="19" t="n"/>
       <c r="Q14" s="15" t="n"/>
       <c r="R14" s="15" t="n"/>
@@ -28555,4 +29288,292 @@
   <pageSetup orientation="portrait" paperSize="9"/>
   <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C40"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="37" t="inlineStr">
+        <is>
+          <t>ARTÍCULOS POR AÑO</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="38" t="inlineStr">
+        <is>
+          <t>Año</t>
+        </is>
+      </c>
+      <c r="B2" s="38" t="inlineStr">
+        <is>
+          <t>Cantidad</t>
+        </is>
+      </c>
+      <c r="C2" s="38" t="inlineStr">
+        <is>
+          <t>Porcentaje</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="39" t="n">
+        <v>2025</v>
+      </c>
+      <c r="B3" t="n">
+        <v>1</v>
+      </c>
+      <c r="C3" s="40">
+        <f>B3/B11</f>
+        <v/>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="39" t="n">
+        <v>2024</v>
+      </c>
+      <c r="B4" t="n">
+        <v>1</v>
+      </c>
+      <c r="C4" s="40">
+        <f>B4/B11</f>
+        <v/>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="39" t="n">
+        <v>2023</v>
+      </c>
+      <c r="B5" t="n">
+        <v>4</v>
+      </c>
+      <c r="C5" s="40">
+        <f>B5/B11</f>
+        <v/>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="39" t="n">
+        <v>2022</v>
+      </c>
+      <c r="B6" t="n">
+        <v>1</v>
+      </c>
+      <c r="C6" s="40">
+        <f>B6/B11</f>
+        <v/>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="39" t="n">
+        <v>2019</v>
+      </c>
+      <c r="B7" t="n">
+        <v>2</v>
+      </c>
+      <c r="C7" s="40">
+        <f>B7/B11</f>
+        <v/>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="39" t="n">
+        <v>2017</v>
+      </c>
+      <c r="B8" t="n">
+        <v>1</v>
+      </c>
+      <c r="C8" s="40">
+        <f>B8/B11</f>
+        <v/>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="39" t="n">
+        <v>2012</v>
+      </c>
+      <c r="B9" t="n">
+        <v>1</v>
+      </c>
+      <c r="C9" s="40">
+        <f>B9/B11</f>
+        <v/>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="39" t="n">
+        <v>2006</v>
+      </c>
+      <c r="B10" t="n">
+        <v>1</v>
+      </c>
+      <c r="C10" s="40">
+        <f>B10/B11</f>
+        <v/>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="38" t="inlineStr">
+        <is>
+          <t>Total</t>
+        </is>
+      </c>
+      <c r="B11" s="38" t="n">
+        <v>12</v>
+      </c>
+      <c r="C11" s="38" t="n"/>
+    </row>
+    <row r="31">
+      <c r="A31" s="37" t="inlineStr">
+        <is>
+          <t>ARTÍCULOS POR PAÍS</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="38" t="inlineStr">
+        <is>
+          <t>País</t>
+        </is>
+      </c>
+      <c r="B32" s="38" t="inlineStr">
+        <is>
+          <t>Cantidad</t>
+        </is>
+      </c>
+      <c r="C32" s="38" t="inlineStr">
+        <is>
+          <t>Porcentaje</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="39" t="inlineStr">
+        <is>
+          <t>USA</t>
+        </is>
+      </c>
+      <c r="B33" t="n">
+        <v>4</v>
+      </c>
+      <c r="C33" s="40">
+        <f>B33/B40</f>
+        <v/>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="39" t="inlineStr">
+        <is>
+          <t>China</t>
+        </is>
+      </c>
+      <c r="B34" t="n">
+        <v>2</v>
+      </c>
+      <c r="C34" s="40">
+        <f>B34/B40</f>
+        <v/>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="39" t="inlineStr">
+        <is>
+          <t>India</t>
+        </is>
+      </c>
+      <c r="B35" t="n">
+        <v>2</v>
+      </c>
+      <c r="C35" s="40">
+        <f>B35/B40</f>
+        <v/>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="39" t="inlineStr">
+        <is>
+          <t>Pakistan</t>
+        </is>
+      </c>
+      <c r="B36" t="n">
+        <v>1</v>
+      </c>
+      <c r="C36" s="40">
+        <f>B36/B40</f>
+        <v/>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="39" t="inlineStr">
+        <is>
+          <t>Canada</t>
+        </is>
+      </c>
+      <c r="B37" t="n">
+        <v>1</v>
+      </c>
+      <c r="C37" s="40">
+        <f>B37/B40</f>
+        <v/>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="39" t="inlineStr">
+        <is>
+          <t>No Disponible</t>
+        </is>
+      </c>
+      <c r="B38" t="n">
+        <v>1</v>
+      </c>
+      <c r="C38" s="40">
+        <f>B38/B40</f>
+        <v/>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="39" t="inlineStr">
+        <is>
+          <t>Czech Republic</t>
+        </is>
+      </c>
+      <c r="B39" t="n">
+        <v>1</v>
+      </c>
+      <c r="C39" s="40">
+        <f>B39/B40</f>
+        <v/>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="38" t="inlineStr">
+        <is>
+          <t>Total</t>
+        </is>
+      </c>
+      <c r="B40" s="38" t="n">
+        <v>12</v>
+      </c>
+      <c r="C40" s="38" t="n"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="A31:C31"/>
+  </mergeCells>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>